<commit_message>
añadido "Técnico/Superior" a los catálagos de la plantilla de importación/exportación
Signed-off-by: Rodolfo V. Carmona Noguera <vladcarmona6@gmail.com>
</commit_message>
<xml_diff>
--- a/components/excel/templates/lwr_contacts_es.xlsx
+++ b/components/excel/templates/lwr_contacts_es.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WWWDev\htdocs\lwr\components\excel\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\clac\htdocs\mye\components\excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AB05BB75-9AE0-46C8-887D-52C6B3A331D0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{52EDE69B-8DF1-4D82-A662-8B084D4914A2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="23040" windowHeight="9048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="23040" windowHeight="9045" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="datos" sheetId="4" r:id="rId1"/>
-    <sheet name="catalogos" sheetId="9" state="hidden" r:id="rId2"/>
+    <sheet name="catalogos" sheetId="9" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">datos!$A$2:$B$2</definedName>
@@ -55,9 +55,6 @@
     <t>Secundaria</t>
   </si>
   <si>
-    <t>Superior</t>
-  </si>
-  <si>
     <t>Organización Implementadora</t>
   </si>
   <si>
@@ -268,6 +265,9 @@
   </si>
   <si>
     <t>Organización Perteneciente</t>
+  </si>
+  <si>
+    <t>Técnico/Superior</t>
   </si>
 </sst>
 </file>
@@ -767,35 +767,35 @@
   </sheetPr>
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.5546875" customWidth="1"/>
-    <col min="2" max="2" width="35.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" style="16" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" customWidth="1"/>
-    <col min="10" max="12" width="12.6640625" customWidth="1"/>
-    <col min="13" max="13" width="10.88671875" customWidth="1"/>
+    <col min="1" max="1" width="47.5703125" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="12" width="12.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
     <col min="14" max="15" width="14" customWidth="1"/>
-    <col min="16" max="16" width="14.6640625" customWidth="1"/>
-    <col min="17" max="18" width="13.6640625" customWidth="1"/>
-    <col min="19" max="19" width="13.33203125" customWidth="1"/>
-    <col min="20" max="20" width="18.5546875" customWidth="1"/>
-    <col min="21" max="21" width="15.88671875" customWidth="1"/>
-    <col min="22" max="23" width="17.6640625" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" customWidth="1"/>
+    <col min="17" max="18" width="13.7109375" customWidth="1"/>
+    <col min="19" max="19" width="13.28515625" customWidth="1"/>
+    <col min="20" max="20" width="18.5703125" customWidth="1"/>
+    <col min="21" max="21" width="15.85546875" customWidth="1"/>
+    <col min="22" max="23" width="17.7109375" customWidth="1"/>
     <col min="27" max="27" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="18" t="s">
@@ -815,7 +815,7 @@
       <c r="O1" s="18"/>
       <c r="P1" s="18"/>
       <c r="Q1" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R1" s="20"/>
       <c r="S1" s="20"/>
@@ -824,21 +824,21 @@
       <c r="V1" s="20"/>
       <c r="W1" s="20"/>
     </row>
-    <row r="2" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>1</v>
@@ -850,49 +850,49 @@
         <v>3</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="P2" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="S2" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="T2" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="U2" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="V2" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="W2" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="W2" s="7" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -973,267 +973,267 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="9" width="18" style="11" customWidth="1"/>
-    <col min="10" max="16384" width="11.44140625" style="11"/>
+    <col min="10" max="16384" width="11.42578125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="12"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
       <c r="C3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>18</v>
-      </c>
       <c r="F3" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="12"/>
       <c r="C4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="12"/>
       <c r="D5" s="13" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="12"/>
       <c r="D6" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
       <c r="D7" s="13" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="12"/>
       <c r="F8" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="12"/>
       <c r="F9" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="12"/>
       <c r="F10" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="12"/>
       <c r="F11" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="12"/>
       <c r="F12" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="12"/>
       <c r="F13" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
       <c r="F14" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="12"/>
       <c r="F15" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="12"/>
       <c r="F16" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="12"/>
       <c r="F17" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="12"/>
       <c r="F18" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="12"/>
       <c r="F19" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="12"/>
       <c r="F20" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="12"/>
       <c r="F21" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="12"/>
       <c r="F22" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="12"/>
       <c r="F23" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="12"/>
       <c r="F24" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="12"/>
       <c r="F25" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="12"/>
       <c r="F26" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="12"/>
       <c r="F27" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="14"/>
       <c r="F28" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="14"/>
       <c r="F29" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="14"/>
       <c r="F30" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="14"/>
       <c r="F31" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="11" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F32" s="11" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Añadiendo la opción de "Universidad" en la plantilla de carga de datos Ocultando la pestaña de "catalogos" de la plantilla
</commit_message>
<xml_diff>
--- a/components/excel/templates/lwr_contacts_es.xlsx
+++ b/components/excel/templates/lwr_contacts_es.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\clac\htdocs\mye\components\excel\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\htdocs\mye\components\excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{52EDE69B-8DF1-4D82-A662-8B084D4914A2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D693635-06BA-4607-A094-ECA1F0CA9B4D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="23040" windowHeight="9045" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="23040" windowHeight="9048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="datos" sheetId="4" r:id="rId1"/>
-    <sheet name="catalogos" sheetId="9" r:id="rId2"/>
+    <sheet name="catalogos" sheetId="9" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">datos!$A$2:$B$2</definedName>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>Fecha de Nacimiento</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>Técnico/Superior</t>
+  </si>
+  <si>
+    <t>Universidad</t>
   </si>
 </sst>
 </file>
@@ -767,33 +770,33 @@
   </sheetPr>
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.5703125" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="16" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="12" width="12.7109375" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="47.5546875" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" style="16" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="10" max="12" width="12.6640625" customWidth="1"/>
+    <col min="13" max="13" width="10.88671875" customWidth="1"/>
     <col min="14" max="15" width="14" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" customWidth="1"/>
-    <col min="17" max="18" width="13.7109375" customWidth="1"/>
-    <col min="19" max="19" width="13.28515625" customWidth="1"/>
-    <col min="20" max="20" width="18.5703125" customWidth="1"/>
-    <col min="21" max="21" width="15.85546875" customWidth="1"/>
-    <col min="22" max="23" width="17.7109375" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" customWidth="1"/>
+    <col min="17" max="18" width="13.6640625" customWidth="1"/>
+    <col min="19" max="19" width="13.33203125" customWidth="1"/>
+    <col min="20" max="20" width="18.5546875" customWidth="1"/>
+    <col min="21" max="21" width="15.88671875" customWidth="1"/>
+    <col min="22" max="23" width="17.6640625" customWidth="1"/>
     <col min="27" max="27" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>52</v>
       </c>
@@ -824,7 +827,7 @@
       <c r="V1" s="20"/>
       <c r="W1" s="20"/>
     </row>
-    <row r="2" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -973,17 +976,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="9" width="18" style="11" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="11"/>
+    <col min="10" max="16384" width="11.44140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>68</v>
       </c>
@@ -1012,10 +1015,10 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" s="12"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" s="12"/>
       <c r="C3" s="11" t="s">
         <v>16</v>
@@ -1030,7 +1033,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="12"/>
       <c r="C4" s="11" t="s">
         <v>5</v>
@@ -1045,7 +1048,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" s="12"/>
       <c r="D5" s="13" t="s">
         <v>6</v>
@@ -1057,7 +1060,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" s="12"/>
       <c r="D6" s="13" t="s">
         <v>7</v>
@@ -1069,7 +1072,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" s="12"/>
       <c r="D7" s="13" t="s">
         <v>78</v>
@@ -1081,8 +1084,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" s="12"/>
+      <c r="D8" s="11" t="s">
+        <v>79</v>
+      </c>
       <c r="F8" s="11" t="s">
         <v>25</v>
       </c>
@@ -1090,7 +1096,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" s="12"/>
       <c r="F9" s="11" t="s">
         <v>26</v>
@@ -1099,139 +1105,139 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" s="12"/>
       <c r="F10" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" s="12"/>
       <c r="F11" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="12"/>
       <c r="F12" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" s="12"/>
       <c r="F13" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="12"/>
       <c r="F14" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="12"/>
       <c r="F15" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" s="12"/>
       <c r="F16" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="12"/>
       <c r="F17" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="12"/>
       <c r="F18" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="12"/>
       <c r="F19" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="12"/>
       <c r="F20" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="12"/>
       <c r="F21" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="12"/>
       <c r="F22" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="12"/>
       <c r="F23" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="12"/>
       <c r="F24" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="12"/>
       <c r="F25" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="12"/>
       <c r="F26" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="12"/>
       <c r="F27" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="14"/>
       <c r="F28" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="14"/>
       <c r="F29" s="11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="14"/>
       <c r="F30" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31" s="14"/>
       <c r="F31" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F32" s="11" t="s">
         <v>49</v>
       </c>

</xml_diff>